<commit_message>
Deploy completo: Dashboard ALOCAMA com efeito hover no botão
 Funcionalidades implementadas:
- Dashboard completo com análise de dados Excel
- Gráficos interativos (pizza, barras, linhas)
- Análise por grupos: AXX, PRONEP, Grupo Solar
- Projeções otimistas, realistas e pessimistas
- Efeito hover no botão 'Executar Análise' (pulse + borda azul)
- Sistema de segurança e validação de arquivos
- Loading screen moderno
- Interface responsiva e elegante

 Melhorias técnicas:
- Código otimizado e limpo
- Logging completo
- Validação de segurança
- Configurações centralizadas
- Performance aprimorada

 Dados atualizados:
- Todos os arquivos Excel dos grupos
- Cálculos de faturamento precisos
- Projeções baseadas em dados reais
</commit_message>
<xml_diff>
--- a/GRUPO SOLAR/DOMMUS/2025-06/DOMUS 06 DE 2025 EXCEL.xlsx
+++ b/GRUPO SOLAR/DOMMUS/2025-06/DOMUS 06 DE 2025 EXCEL.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas.missiba\Desktop\projetoalocama\GRUPO SOLAR\DOMMUS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas.missiba\Desktop\projetoalocama\GRUPO SOLAR\DOMMUS\2025-06\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D4222C6-3E8E-409D-ABB2-4A748E2DD90D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D4BA040-49EA-4C97-AA36-E5567A319AF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1008,8 +1008,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y90"/>
   <sheetViews>
-    <sheetView tabSelected="1" showOutlineSymbols="0" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
+    <sheetView tabSelected="1" showOutlineSymbols="0" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="Y60" sqref="Y60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5" x14ac:dyDescent="0.25"/>

</xml_diff>